<commit_message>
feat(reader): now the reader add models to database
</commit_message>
<xml_diff>
--- a/reader/output/aguas_andinas_bills.xlsx
+++ b/reader/output/aguas_andinas_bills.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -459,11 +459,6 @@
           <t>year</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>month_year</t>
-        </is>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -476,23 +471,14 @@
           <t>461384-8</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>149948</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>February</t>
-        </is>
+      <c r="C2" t="n">
+        <v>149948</v>
+      </c>
+      <c r="D2" t="n">
+        <v>1</v>
       </c>
       <c r="E2" t="n">
         <v>2025</v>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>02-2025</t>
-        </is>
       </c>
     </row>
     <row r="3">
@@ -506,23 +492,14 @@
           <t>461384-8</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>237310</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>March</t>
-        </is>
+      <c r="C3" t="n">
+        <v>237310</v>
+      </c>
+      <c r="D3" t="n">
+        <v>2</v>
       </c>
       <c r="E3" t="n">
         <v>2023</v>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>03-2023</t>
-        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>